<commit_message>
add sources data and definitions
</commit_message>
<xml_diff>
--- a/01_Datasources/ref_memberstates.xlsx
+++ b/01_Datasources/ref_memberstates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lehlohonolo Makoti\Documents\Learning &amp; Dev\Consultant Analytics\SADC Analytics\Resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lehlohonolo Makoti\Documents\Learning &amp; Dev\Data Work Portfolio\UN Data Analytics Portfolio\SDG5-Gender-Equality\01_Datasources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A30FFB18-DC5C-40A4-9DBD-6606FAC2429B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F459C-EB41-449A-AD0A-B930B5C55196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C62AE921-720A-41A9-8EBB-7C4AFDBC9EBD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C62AE921-720A-41A9-8EBB-7C4AFDBC9EBD}"/>
   </bookViews>
   <sheets>
     <sheet name="sadc_countries" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
add dashboard and documentation
</commit_message>
<xml_diff>
--- a/01_Datasources/ref_memberstates.xlsx
+++ b/01_Datasources/ref_memberstates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lehlohonolo Makoti\Documents\Learning &amp; Dev\Data Work Portfolio\UN Data Analytics Portfolio\SDG5-Gender-Equality\01_Datasources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F2F459C-EB41-449A-AD0A-B930B5C55196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9B9555-6816-4795-9364-FB1BC4175773}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21840" xr2:uid="{C62AE921-720A-41A9-8EBB-7C4AFDBC9EBD}"/>
+    <workbookView xWindow="1860" yWindow="1860" windowWidth="28800" windowHeight="15885" xr2:uid="{C62AE921-720A-41A9-8EBB-7C4AFDBC9EBD}"/>
   </bookViews>
   <sheets>
     <sheet name="sadc_countries" sheetId="1" r:id="rId1"/>
@@ -192,7 +192,7 @@
     <t>ZWE</t>
   </si>
   <si>
-    <t>Congo</t>
+    <t>DRC</t>
   </si>
 </sst>
 </file>
@@ -562,7 +562,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>